<commit_message>
Changed algorithm of adding modifiers in the patcher
- added IsAbsoluteProbability property instead of IsNormalizedProbability;
- the algorithm was rewritten to make chances of modifiers more predictable;
- fixed some errors;
- removed NST modififer;
- changed modifiers presets;
</commit_message>
<xml_diff>
--- a/docs/UD_Modifiers.xlsx
+++ b/docs/UD_Modifiers.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Service" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Modifier with Presets'!$B$5:$AF$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Modifier with Presets'!$B$5:$AF$48</definedName>
     <definedName name="List_Boolean">Service!$B$2:$B$3</definedName>
     <definedName name="List_ModOutcomes">Service!$F$2:$F$19</definedName>
     <definedName name="List_ModTriggers">Service!$D$2:$D$21</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="347">
   <si>
     <t>Name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Base</t>
-  </si>
-  <si>
-    <t>IsNorm</t>
   </si>
   <si>
     <t>Severity</t>
@@ -900,34 +897,13 @@
     <t>This modifier is only added to devices that have an alternate way to escape (see ESC tag)</t>
   </si>
   <si>
-    <t>No stealing</t>
-  </si>
-  <si>
-    <t>Punishes attempted stealing by summoning heavy bondage</t>
-  </si>
-  <si>
-    <t>NST</t>
-  </si>
-  <si>
     <t>ItemObtain</t>
-  </si>
-  <si>
-    <t>1,10,10,24,1,,,1,R</t>
-  </si>
-  <si>
-    <t>1,25,25,12,1,,,1,R</t>
-  </si>
-  <si>
-    <t>1,50,50,8,1,,,1,R</t>
   </si>
   <si>
     <t>zad_DeviousBondageMittens
 zad_DeviousHeavyBondage</t>
   </si>
   <si>
-    <t>UD_Modifier_NST_Form1Vars</t>
-  </si>
-  <si>
     <t>Sweet Roll Thief</t>
   </si>
   <si>
@@ -1107,6 +1083,9 @@
   </si>
   <si>
     <t>ModPreset1_CheapLocks</t>
+  </si>
+  <si>
+    <t>IsAbs</t>
   </si>
 </sst>
 </file>
@@ -1367,6 +1346,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1379,20 +1370,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1681,13 +1660,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AF49"/>
+  <dimension ref="B2:AF48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="V26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomRight" activeCell="X49" sqref="X49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,137 +1699,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="32" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF2" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="30" t="s">
-        <v>282</v>
-      </c>
-      <c r="AF2" s="30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="28" t="s">
-        <v>350</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" s="32" t="s">
+      <c r="I3" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="32"/>
+      <c r="N3" s="25"/>
       <c r="O3" s="34" t="s">
         <v>8</v>
       </c>
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="T3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="U3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="30" t="s">
+      <c r="V3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="V3" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="32" t="s">
+      <c r="W3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="32"/>
+      <c r="X3" s="25"/>
       <c r="Y3" s="35" t="s">
         <v>15</v>
       </c>
       <c r="Z3" s="35"/>
-      <c r="AA3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31"/>
+      <c r="AA3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="33"/>
     </row>
     <row r="4" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="32"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1866,11 +1845,11 @@
       <c r="Q4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
       <c r="W4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1881,22 +1860,22 @@
         <v>16</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>17</v>
+        <v>346</v>
       </c>
       <c r="AA4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AC4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
+        <v>20</v>
+      </c>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
     </row>
     <row r="5" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -1995,46 +1974,46 @@
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="O6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="Q6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="W6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y6" s="8">
         <v>0.5</v>
@@ -2049,51 +2028,51 @@
         <v>0.2</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="K7" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O7" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="P7" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="Q7" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="Q7" s="17" t="s">
-        <v>235</v>
-      </c>
       <c r="W7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y7" s="8">
         <v>0.15</v>
@@ -2108,60 +2087,60 @@
         <v>0.2</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="K8" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O8" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="P8" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="Q8" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="Q8" s="17" t="s">
-        <v>229</v>
-      </c>
       <c r="W8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y8" s="8">
         <v>0.25</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA8" s="9">
         <v>0</v>
@@ -2170,21 +2149,21 @@
         <v>0.2</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>58</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -2212,48 +2191,48 @@
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="F10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="Q10" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="Q10" s="17" t="s">
-        <v>67</v>
-      </c>
       <c r="W10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y10" s="8">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA10" s="9">
         <v>0</v>
@@ -2262,54 +2241,54 @@
         <v>0.2</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="F11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="17" t="s">
+      <c r="P11" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="Q11" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="W11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y11" s="8">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>38</v>
@@ -2321,60 +2300,60 @@
         <v>0.2</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="F12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O12" s="17" t="s">
+      <c r="P12" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="Q12" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="Q12" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="W12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y12" s="8">
         <v>0.25</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA12" s="9">
         <v>0</v>
@@ -2383,54 +2362,54 @@
         <v>0.2</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="P13" s="17" t="s">
+      <c r="Q13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Q13" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="W13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y13" s="8">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>38</v>
@@ -2442,60 +2421,60 @@
         <v>0.2</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="P14" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="P14" s="17" t="s">
+      <c r="Q14" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Q14" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="W14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y14" s="8">
         <v>0.25</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA14" s="9">
         <v>0</v>
@@ -2504,35 +2483,35 @@
         <v>0.2</v>
       </c>
       <c r="AC14" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="G15" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="O15" s="17">
         <v>1</v>
@@ -2544,10 +2523,10 @@
         <v>0.05</v>
       </c>
       <c r="W15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y15" s="8">
         <v>0.5</v>
@@ -2562,35 +2541,35 @@
         <v>0.3</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="G16" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O16" s="17">
         <v>5</v>
@@ -2602,16 +2581,16 @@
         <v>50</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y16" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA16" s="9">
         <v>0</v>
@@ -2620,57 +2599,57 @@
         <v>0.2</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="K17" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O17" s="17" t="s">
+      <c r="P17" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="P17" s="17" t="s">
+      <c r="Q17" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="Q17" s="17" t="s">
+      <c r="S17" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="S17" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="W17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y17" s="8">
         <v>0.25</v>
@@ -2685,51 +2664,51 @@
         <v>0.2</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O18" s="17" t="s">
+      <c r="P18" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="Q18" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="Q18" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="W18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y18" s="8">
         <v>0.25</v>
@@ -2744,47 +2723,47 @@
         <v>0.2</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="F19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="21" t="s">
         <v>116</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>117</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="K19" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O19" s="17" t="s">
+      <c r="P19" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="P19" s="17" t="s">
+      <c r="Q19" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="Q19" s="17" t="s">
-        <v>122</v>
-      </c>
       <c r="W19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X19" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X19" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y19" s="8">
         <v>0.15</v>
@@ -2799,30 +2778,30 @@
         <v>0.2</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -2848,21 +2827,21 @@
     </row>
     <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="G21" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -2886,54 +2865,54 @@
       <c r="AD21" s="11"/>
       <c r="AE21" s="11"/>
       <c r="AF21" s="5" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="S22" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O22" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="P22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q22" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="S22" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="W22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y22" s="8">
         <v>0.15</v>
@@ -2950,52 +2929,52 @@
     </row>
     <row r="23" spans="2:32" ht="72" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="O23" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="K23" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="O23" s="17" t="s">
+      <c r="P23" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="P23" s="17" t="s">
+      <c r="Q23" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="S23" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="S23" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="W23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y23" s="8">
         <v>0.25</v>
@@ -3010,54 +2989,54 @@
         <v>0.2</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O24" s="17" t="s">
+      <c r="P24" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="P24" s="17" t="s">
+      <c r="Q24" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="Q24" s="17" t="s">
-        <v>159</v>
-      </c>
       <c r="S24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y24" s="8">
         <v>0.25</v>
@@ -3072,57 +3051,57 @@
         <v>0.2</v>
       </c>
       <c r="AC24" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="G25" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="O25" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N25" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="O25" s="17" t="s">
+      <c r="P25" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="Q25" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="Q25" s="17" t="s">
+      <c r="S25" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="S25" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="W25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y25" s="8">
         <v>0.15</v>
@@ -3139,52 +3118,52 @@
     </row>
     <row r="26" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="G26" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="O26" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N26" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="O26" s="17" t="s">
+      <c r="P26" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="P26" s="17" t="s">
+      <c r="Q26" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="Q26" s="17" t="s">
-        <v>177</v>
-      </c>
       <c r="S26" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y26" s="8">
         <v>0.15</v>
@@ -3201,48 +3180,48 @@
     </row>
     <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>181</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M27" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N27" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="R27" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="R27" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="W27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X27" s="5" t="s">
         <v>38</v>
       </c>
       <c r="Y27" s="8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Z27" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA27" s="9">
         <v>0</v>
@@ -3251,66 +3230,66 @@
         <v>0.2</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AD27" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G28" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="K28" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N28" s="5" t="s">
+      <c r="O28" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="O28" s="17" t="s">
+      <c r="P28" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="P28" s="17" t="s">
+      <c r="Q28" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="Q28" s="17" t="s">
+      <c r="S28" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S28" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="W28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y28" s="8">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="Z28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA28" s="9">
         <v>0</v>
@@ -3321,52 +3300,52 @@
     </row>
     <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="G29" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G29" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N29" s="5" t="s">
+      <c r="O29" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="O29" s="17" t="s">
+      <c r="P29" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="P29" s="17" t="s">
+      <c r="Q29" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="Q29" s="17" t="s">
+      <c r="S29" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="S29" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="W29" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y29" s="8">
         <v>0.15</v>
@@ -3383,58 +3362,58 @@
     </row>
     <row r="30" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K30" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="O30" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K30" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M30" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="O30" s="17" t="s">
+      <c r="P30" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q30" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="P30" s="17" t="s">
+      <c r="S30" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="Q30" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="W30" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X30" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y30" s="8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Z30" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA30" s="9">
         <v>0</v>
@@ -3443,51 +3422,51 @@
         <v>0.2</v>
       </c>
       <c r="AC30" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G31" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="K31" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O31" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="P31" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="P31" s="17" t="s">
+      <c r="Q31" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="Q31" s="17" t="s">
-        <v>238</v>
-      </c>
       <c r="W31" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X31" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y31" s="8">
         <v>0.05</v>
@@ -3502,63 +3481,63 @@
         <v>0.2</v>
       </c>
       <c r="AC31" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD31" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="AD31" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="K32" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O32" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="P32" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="P32" s="17" t="s">
+      <c r="Q32" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="Q32" s="17" t="s">
-        <v>232</v>
-      </c>
       <c r="W32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y32" s="8">
         <v>0.05</v>
       </c>
       <c r="Z32" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA32" s="9">
         <v>0</v>
@@ -3567,54 +3546,54 @@
         <v>0.2</v>
       </c>
       <c r="AC32" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD32" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="AD32" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P33" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W33" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X33" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y33" s="8">
         <v>0.05</v>
@@ -3629,63 +3608,63 @@
         <v>0.2</v>
       </c>
       <c r="AC33" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD33" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="AD33" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="K34" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="K34" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="P34" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q34" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="P34" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q34" s="17" t="s">
-        <v>224</v>
-      </c>
       <c r="W34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y34" s="8">
         <v>0.05</v>
       </c>
       <c r="Z34" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA34" s="9">
         <v>0</v>
@@ -3694,54 +3673,54 @@
         <v>0.2</v>
       </c>
       <c r="AC34" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD34" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="AD34" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="G35" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="K35" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O35" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="P35" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="P35" s="17" t="s">
+      <c r="Q35" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="Q35" s="17" t="s">
-        <v>235</v>
-      </c>
       <c r="W35" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X35" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y35" s="8">
         <v>0.15</v>
@@ -3756,60 +3735,60 @@
         <v>0.2</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="G36" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J36" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="K36" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O36" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="P36" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="P36" s="17" t="s">
+      <c r="Q36" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="Q36" s="17" t="s">
-        <v>229</v>
-      </c>
       <c r="W36" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y36" s="8">
         <v>0.25</v>
       </c>
       <c r="Z36" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA36" s="9">
         <v>0</v>
@@ -3818,30 +3797,30 @@
         <v>0.2</v>
       </c>
       <c r="AC36" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="G37" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
@@ -3867,49 +3846,49 @@
     </row>
     <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="G38" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="P38" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q38" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="S38" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="K38" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="P38" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q38" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="S38" s="5" t="s">
-        <v>252</v>
-      </c>
       <c r="W38" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X38" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y38" s="8">
         <v>0.15</v>
@@ -3924,51 +3903,54 @@
         <v>0.2</v>
       </c>
       <c r="AC38" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="F39" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="G39" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="O39" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="K39" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O39" s="17" t="s">
+      <c r="P39" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="P39" s="17" t="s">
+      <c r="Q39" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="Q39" s="17" t="s">
-        <v>263</v>
-      </c>
       <c r="W39" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X39" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y39" s="8">
         <v>0.05</v>
@@ -3983,53 +3965,56 @@
         <v>0.2</v>
       </c>
       <c r="AC39" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="G40" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="K40" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="O40" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="K40" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O40" s="17" t="s">
+      <c r="P40" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="P40" s="17" t="s">
+      <c r="Q40" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="Q40" s="17" t="s">
-        <v>270</v>
-      </c>
       <c r="W40" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X40" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y40" s="8">
         <v>0.1</v>
       </c>
       <c r="Z40" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA40" s="9">
         <v>0</v>
@@ -4038,54 +4023,54 @@
         <v>0.2</v>
       </c>
       <c r="AF40" s="5" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I41" s="5" t="s">
+      <c r="J41" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>275</v>
-      </c>
       <c r="K41" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P41" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q41" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W41" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X41" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y41" s="8">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="Z41" s="5" t="s">
         <v>38</v>
@@ -4097,54 +4082,54 @@
         <v>0.2</v>
       </c>
       <c r="AC41" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF41" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="G42" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="K42" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O42" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="P42" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W42" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X42" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X42" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y42" s="8">
         <v>0.05</v>
@@ -4159,45 +4144,45 @@
         <v>0.2</v>
       </c>
       <c r="AC42" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AE42" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="AF42" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="AF42" s="5" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="43" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N43" s="15" t="s">
         <v>285</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="G43" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K43" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N43" s="15" t="s">
-        <v>292</v>
       </c>
       <c r="O43" s="17" t="s">
         <v>289</v>
@@ -4209,13 +4194,10 @@
         <v>291</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>168</v>
+        <v>292</v>
       </c>
       <c r="W43" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X43" s="5" t="s">
         <v>38</v>
@@ -4232,37 +4214,40 @@
       <c r="AB43" s="10">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="44" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AC43" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="F44" s="5" t="s">
+      <c r="G44" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K44" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="K44" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="15" t="s">
-        <v>292</v>
       </c>
       <c r="O44" s="17" t="s">
         <v>297</v>
@@ -4273,20 +4258,17 @@
       <c r="Q44" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="R44" s="5" t="s">
-        <v>300</v>
-      </c>
       <c r="W44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="X44" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="Y44" s="8">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="Z44" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA44" s="9">
         <v>0</v>
@@ -4295,138 +4277,138 @@
         <v>0.2</v>
       </c>
       <c r="AC44" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="G45" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="G45" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="O45" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="P45" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q45" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="W45" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X45" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y45" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="Z45" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="AC45" s="5" t="s">
-        <v>260</v>
-      </c>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="11"/>
     </row>
     <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K46" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="O46" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="P46" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="Q46" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
-      <c r="T46" s="11"/>
-      <c r="U46" s="11"/>
-      <c r="V46" s="11"/>
-      <c r="W46" s="11"/>
-      <c r="X46" s="11"/>
-      <c r="Y46" s="11"/>
-      <c r="Z46" s="11"/>
-      <c r="AA46" s="11"/>
-      <c r="AB46" s="11"/>
-      <c r="AC46" s="11"/>
-      <c r="AD46" s="11"/>
-      <c r="AE46" s="11"/>
+      <c r="W46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y46" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="Z46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC46" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="47" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>315</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H47" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K47" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M47" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K47" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>319</v>
       </c>
       <c r="O47" s="17" t="s">
         <v>316</v>
@@ -4438,16 +4420,16 @@
         <v>318</v>
       </c>
       <c r="W47" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X47" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="X47" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="Y47" s="8">
         <v>0.05</v>
       </c>
       <c r="Z47" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA47" s="9">
         <v>0</v>
@@ -4456,60 +4438,63 @@
         <v>0.2</v>
       </c>
       <c r="AC47" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>323</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>321</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="K48" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="O48" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="O48" s="17" t="s">
+      <c r="P48" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q48" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="P48" s="17" t="s">
+      <c r="S48" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="Q48" s="17" t="s">
-        <v>326</v>
-      </c>
       <c r="W48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X48" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="X48" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="Y48" s="8">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="Z48" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA48" s="9">
         <v>0</v>
@@ -4517,88 +4502,10 @@
       <c r="AB48" s="10">
         <v>0.2</v>
       </c>
-      <c r="AC48" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B49" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="G49" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N49" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="O49" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="P49" s="17" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q49" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="S49" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="W49" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X49" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y49" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="Z49" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB49" s="10">
-        <v>0.2</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AF49"/>
+  <autoFilter ref="B5:AF48"/>
   <mergeCells count="27">
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="K2:AD2"/>
-    <mergeCell ref="K3:K4"/>
     <mergeCell ref="AF2:AF4"/>
     <mergeCell ref="AE2:AE4"/>
     <mergeCell ref="D2:F2"/>
@@ -4613,6 +4520,19 @@
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="K2:AD2"/>
+    <mergeCell ref="K3:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4635,173 +4555,173 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="F5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F10" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F11" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="F15" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="F16" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated documentation, added new modifier
- updated documentation in UD_Modifier.xlsx and added new "Combo Matrix" list;
- added new modifier LCOL - Liquid Collector (Orgasm -> Add Potion) for belt devices.
</commit_message>
<xml_diff>
--- a/docs/UD_Modifiers.xlsx
+++ b/docs/UD_Modifiers.xlsx
@@ -12,13 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13272"/>
   </bookViews>
   <sheets>
-    <sheet name="Modifier with Presets" sheetId="1" r:id="rId1"/>
-    <sheet name="Service" sheetId="2" r:id="rId2"/>
+    <sheet name="Modifiers &amp; Presets" sheetId="1" r:id="rId1"/>
+    <sheet name="Combo Matrix" sheetId="3" r:id="rId2"/>
+    <sheet name="Service" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Modifier with Presets'!$B$5:$AF$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Modifiers &amp; Presets'!$B$5:$AF$48</definedName>
     <definedName name="List_Boolean">Service!$B$2:$B$3</definedName>
-    <definedName name="List_ModOutcomes">Service!$F$2:$F$19</definedName>
+    <definedName name="List_ModOutcomes">Service!$F$2:$F$17</definedName>
     <definedName name="List_ModTriggers">Service!$D$2:$D$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="405">
   <si>
     <t>Name</t>
   </si>
@@ -671,9 +672,6 @@
     <t>2,10,10,1,,,,1,1,1</t>
   </si>
   <si>
-    <t>AlcoholicDrinksList</t>
-  </si>
-  <si>
     <t>This device materializes alcoholic drinks magically from time to time</t>
   </si>
   <si>
@@ -946,9 +944,6 @@
     <t>Locations Discovered,0,100,,,,,B,0.5,1</t>
   </si>
   <si>
-    <t>Enchanted</t>
-  </si>
-  <si>
     <t>ENCH</t>
   </si>
   <si>
@@ -1086,6 +1081,437 @@
   </si>
   <si>
     <t>IsAbs</t>
+  </si>
+  <si>
+    <t>Triggers/Outcomes</t>
+  </si>
+  <si>
+    <t>LCOL</t>
+  </si>
+  <si>
+    <t>Liquid Collector</t>
+  </si>
+  <si>
+    <t>The device has the ability to collect your secretions and produce bottles of potions</t>
+  </si>
+  <si>
+    <t>zad_DeviousBelt</t>
+  </si>
+  <si>
+    <t>0,100,0,1,,,,1</t>
+  </si>
+  <si>
+    <t>0,25,0,1,,,,1,1,1</t>
+  </si>
+  <si>
+    <t>UD_Modifier_LCOL_Form2Vars</t>
+  </si>
+  <si>
+    <t>The device demands a goo for each escape attempt</t>
+  </si>
+  <si>
+    <t>Demands goo</t>
+  </si>
+  <si>
+    <t>ITEM-</t>
+  </si>
+  <si>
+    <t>GOO</t>
+  </si>
+  <si>
+    <t>1,1,0,0</t>
+  </si>
+  <si>
+    <t>1,3,0,0</t>
+  </si>
+  <si>
+    <t>UD_Modifier_GOO_Form1Vars</t>
+  </si>
+  <si>
+    <t>UD_Modifier_ALCO_Form2Vars</t>
+  </si>
+  <si>
+    <t>ENCH1</t>
+  </si>
+  <si>
+    <t>ENCH0</t>
+  </si>
+  <si>
+    <t>Enchantment</t>
+  </si>
+  <si>
+    <t>ModPreset3</t>
+  </si>
+  <si>
+    <t>Health Enchantment</t>
+  </si>
+  <si>
+    <t>UD_Modifier_ENCH1_Form1Vars</t>
+  </si>
+  <si>
+    <t>zad_DeviousCorset
+zad_DeviousSuit
+zad_DeviousHarness</t>
+  </si>
+  <si>
+    <t>Stamina Enchantment</t>
+  </si>
+  <si>
+    <t>zad_DeviousBoots
+zad_DeviousLegCuffs
+zad_DeviousPetSuit</t>
+  </si>
+  <si>
+    <t>Magicka Enchantment</t>
+  </si>
+  <si>
+    <t>UD_Modifier_ENCH3_Form1Vars</t>
+  </si>
+  <si>
+    <t>UD_Modifier_ENCH2_Form1Vars</t>
+  </si>
+  <si>
+    <t>zad_DeviousBlindfold
+zad_DeviousGag
+zad_DeviousHood</t>
+  </si>
+  <si>
+    <t>Block
+Minigame</t>
+  </si>
+  <si>
+    <t>Activate
+Device</t>
+  </si>
+  <si>
+    <t>Decrease
+Durability</t>
+  </si>
+  <si>
+    <t>Restore
+Durability</t>
+  </si>
+  <si>
+    <t>Unlock
+Device</t>
+  </si>
+  <si>
+    <t>Remove
+Item</t>
+  </si>
+  <si>
+    <t>4,5,5,0,,,,1,L</t>
+  </si>
+  <si>
+    <t>2,10,5,0,,,,1,L</t>
+  </si>
+  <si>
+    <t>1,20,10,1,,,,1,L</t>
+  </si>
+  <si>
+    <t>1,15,5,0,,,,1,L</t>
+  </si>
+  <si>
+    <t>A1_EVOLUTION</t>
+  </si>
+  <si>
+    <t>A1_MANIFEST</t>
+  </si>
+  <si>
+    <t>A1_WAR_REWARD</t>
+  </si>
+  <si>
+    <t>A1_MAGE_PUNISH
+A2_MAGE_PUNISH</t>
+  </si>
+  <si>
+    <t>A1_THIEF_PUNISH
+A3_THIEF_PUNISH</t>
+  </si>
+  <si>
+    <t>A2_WAR_PUNISH
+A3_WAR_PUNISH</t>
+  </si>
+  <si>
+    <t>A1_MAGE_WARN
+A2_MAGE_WARN</t>
+  </si>
+  <si>
+    <t>A1_THIEF_WARN
+A3_THIEF_WARN</t>
+  </si>
+  <si>
+    <t>A2_WAR_WARN
+A3_WAR_WARN</t>
+  </si>
+  <si>
+    <t>A3_MAGE_REWARD</t>
+  </si>
+  <si>
+    <t>A2_THIEF_REWARD</t>
+  </si>
+  <si>
+    <t>A2_EVOLUTION</t>
+  </si>
+  <si>
+    <t>A3_EVOLUTION</t>
+  </si>
+  <si>
+    <t>A3_MANIFEST</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NKL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+A2_MANIFEST</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OREG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OMREG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AA_REGEN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NSPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NWD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>THS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>POIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NLP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NRE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TREG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TMREG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BOLD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Modifiers have presets for the Patcher and can appear on a random device;
+A*_ - Modifiers are used on Abadon armor</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1122,7 +1548,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1168,6 +1594,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,7 +1706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1352,6 +1784,39 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1378,6 +1843,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1660,13 +2131,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AF48"/>
+  <dimension ref="B2:AF53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="V26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X49" sqref="X49"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,11 +2152,13 @@
     <col min="9" max="9" width="22" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.5546875" style="5" customWidth="1"/>
     <col min="14" max="14" width="24.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="31" style="17" customWidth="1"/>
-    <col min="18" max="22" width="26.21875" style="5" customWidth="1"/>
+    <col min="18" max="18" width="28.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="26.21875" style="5" customWidth="1"/>
     <col min="23" max="24" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
@@ -1699,137 +2172,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF2" s="27" t="s">
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF2" s="38" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="32" t="s">
-        <v>342</v>
-      </c>
-      <c r="E3" s="25" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="37"/>
+      <c r="K3" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="37"/>
+      <c r="O3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="27" t="s">
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="S3" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="T3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="V3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="W3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="35" t="s">
+      <c r="X3" s="37"/>
+      <c r="Y3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="25" t="s">
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25" t="s">
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="33"/>
-      <c r="AF3" s="33"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
     </row>
     <row r="4" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="25"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="37"/>
       <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1845,11 +2318,11 @@
       <c r="Q4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
       <c r="W4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1860,7 +2333,7 @@
         <v>16</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AA4" s="6" t="s">
         <v>16</v>
@@ -1874,8 +2347,8 @@
       <c r="AD4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
     </row>
     <row r="5" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -2016,7 +2489,7 @@
         <v>38</v>
       </c>
       <c r="Y6" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>38</v>
@@ -2060,13 +2533,13 @@
         <v>24</v>
       </c>
       <c r="O7" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="P7" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="Q7" s="17" t="s">
         <v>233</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>234</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>37</v>
@@ -2116,19 +2589,19 @@
         <v>89</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="O8" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="P8" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="Q8" s="17" t="s">
         <v>227</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>228</v>
       </c>
       <c r="W8" s="5" t="s">
         <v>37</v>
@@ -2208,7 +2681,7 @@
         <v>61</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>24</v>
@@ -2276,10 +2749,10 @@
         <v>73</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>74</v>
+        <v>383</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="W11" s="5" t="s">
         <v>37</v>
@@ -2288,7 +2761,7 @@
         <v>37</v>
       </c>
       <c r="Y11" s="8">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>38</v>
@@ -2350,7 +2823,7 @@
         <v>37</v>
       </c>
       <c r="Y12" s="8">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>37</v>
@@ -2394,13 +2867,13 @@
         <v>24</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>73</v>
+        <v>380</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>81</v>
+        <v>381</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>82</v>
+        <v>382</v>
       </c>
       <c r="W13" s="5" t="s">
         <v>37</v>
@@ -2409,7 +2882,7 @@
         <v>37</v>
       </c>
       <c r="Y13" s="8">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>38</v>
@@ -2471,7 +2944,7 @@
         <v>37</v>
       </c>
       <c r="Y14" s="8">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="Z14" s="5" t="s">
         <v>37</v>
@@ -2529,7 +3002,7 @@
         <v>37</v>
       </c>
       <c r="Y15" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z15" s="5" t="s">
         <v>38</v>
@@ -2544,7 +3017,7 @@
         <v>86</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.3">
@@ -2652,7 +3125,7 @@
         <v>38</v>
       </c>
       <c r="Y17" s="8">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Z17" s="5" t="s">
         <v>38</v>
@@ -2865,7 +3338,7 @@
       <c r="AD21" s="11"/>
       <c r="AE21" s="11"/>
       <c r="AF21" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.3">
@@ -3365,7 +3838,7 @@
         <v>205</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>204</v>
@@ -3389,7 +3862,7 @@
         <v>24</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O30" s="17" t="s">
         <v>206</v>
@@ -3401,7 +3874,7 @@
         <v>207</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>209</v>
+        <v>360</v>
       </c>
       <c r="W30" s="5" t="s">
         <v>37</v>
@@ -3427,13 +3900,13 @@
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>30</v>
@@ -3445,7 +3918,7 @@
         <v>47</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>88</v>
@@ -3454,13 +3927,13 @@
         <v>24</v>
       </c>
       <c r="O31" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="P31" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="P31" s="17" t="s">
+      <c r="Q31" s="17" t="s">
         <v>236</v>
-      </c>
-      <c r="Q31" s="17" t="s">
-        <v>237</v>
       </c>
       <c r="W31" s="5" t="s">
         <v>37</v>
@@ -3481,21 +3954,21 @@
         <v>0.2</v>
       </c>
       <c r="AC31" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD31" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="AD31" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>30</v>
@@ -3507,25 +3980,25 @@
         <v>47</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K32" s="24" t="s">
         <v>89</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>53</v>
       </c>
       <c r="O32" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="P32" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="P32" s="17" t="s">
+      <c r="Q32" s="17" t="s">
         <v>230</v>
-      </c>
-      <c r="Q32" s="17" t="s">
-        <v>231</v>
       </c>
       <c r="W32" s="5" t="s">
         <v>37</v>
@@ -3546,21 +4019,21 @@
         <v>0.2</v>
       </c>
       <c r="AC32" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD32" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="AD32" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>30</v>
@@ -3572,7 +4045,7 @@
         <v>47</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K33" s="23" t="s">
         <v>88</v>
@@ -3581,13 +4054,13 @@
         <v>24</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P33" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="W33" s="5" t="s">
         <v>37</v>
@@ -3608,21 +4081,21 @@
         <v>0.2</v>
       </c>
       <c r="AC33" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD33" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="AD33" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>30</v>
@@ -3634,25 +4107,25 @@
         <v>47</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K34" s="24" t="s">
         <v>89</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>87</v>
       </c>
       <c r="O34" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P34" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="P34" s="17" t="s">
-        <v>225</v>
-      </c>
       <c r="Q34" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W34" s="5" t="s">
         <v>37</v>
@@ -3673,21 +4146,21 @@
         <v>0.2</v>
       </c>
       <c r="AC34" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD34" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="AD34" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>30</v>
@@ -3708,13 +4181,13 @@
         <v>24</v>
       </c>
       <c r="O35" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="P35" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="P35" s="17" t="s">
+      <c r="Q35" s="17" t="s">
         <v>233</v>
-      </c>
-      <c r="Q35" s="17" t="s">
-        <v>234</v>
       </c>
       <c r="W35" s="5" t="s">
         <v>37</v>
@@ -3735,18 +4208,18 @@
         <v>0.2</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>30</v>
@@ -3764,19 +4237,19 @@
         <v>89</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>87</v>
       </c>
       <c r="O36" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="P36" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="P36" s="17" t="s">
+      <c r="Q36" s="17" t="s">
         <v>227</v>
-      </c>
-      <c r="Q36" s="17" t="s">
-        <v>228</v>
       </c>
       <c r="W36" s="5" t="s">
         <v>37</v>
@@ -3797,18 +4270,18 @@
         <v>0.2</v>
       </c>
       <c r="AC36" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="G37" s="23" t="s">
         <v>30</v>
@@ -3846,13 +4319,13 @@
     </row>
     <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="G38" s="23" t="s">
         <v>30</v>
@@ -3864,7 +4337,7 @@
         <v>146</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K38" s="23" t="s">
         <v>88</v>
@@ -3873,16 +4346,16 @@
         <v>24</v>
       </c>
       <c r="O38" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="P38" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="P38" s="17" t="s">
+      <c r="Q38" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="Q38" s="17" t="s">
-        <v>254</v>
-      </c>
       <c r="S38" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W38" s="5" t="s">
         <v>37</v>
@@ -3903,18 +4376,18 @@
         <v>0.2</v>
       </c>
       <c r="AC38" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>257</v>
-      </c>
       <c r="F39" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39" s="23" t="s">
         <v>30</v>
@@ -3923,10 +4396,10 @@
         <v>46</v>
       </c>
       <c r="I39" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="K39" s="23" t="s">
         <v>88</v>
@@ -3938,13 +4411,13 @@
         <v>168</v>
       </c>
       <c r="O39" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="P39" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="P39" s="17" t="s">
+      <c r="Q39" s="17" t="s">
         <v>261</v>
-      </c>
-      <c r="Q39" s="17" t="s">
-        <v>262</v>
       </c>
       <c r="W39" s="5" t="s">
         <v>37</v>
@@ -3965,26 +4438,26 @@
         <v>0.2</v>
       </c>
       <c r="AC39" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>265</v>
-      </c>
       <c r="G40" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K40" s="23" t="s">
         <v>88</v>
@@ -3996,13 +4469,13 @@
         <v>168</v>
       </c>
       <c r="O40" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="P40" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="P40" s="17" t="s">
+      <c r="Q40" s="17" t="s">
         <v>268</v>
-      </c>
-      <c r="Q40" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="W40" s="19" t="s">
         <v>38</v>
@@ -4023,18 +4496,18 @@
         <v>0.2</v>
       </c>
       <c r="AF40" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G41" s="23" t="s">
         <v>30</v>
@@ -4043,10 +4516,10 @@
         <v>46</v>
       </c>
       <c r="I41" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="K41" s="23" t="s">
         <v>88</v>
@@ -4082,21 +4555,21 @@
         <v>0.2</v>
       </c>
       <c r="AC41" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF41" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="G42" s="23" t="s">
         <v>30</v>
@@ -4105,10 +4578,10 @@
         <v>27</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>88</v>
@@ -4117,13 +4590,13 @@
         <v>24</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P42" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="W42" s="5" t="s">
         <v>37</v>
@@ -4144,36 +4617,36 @@
         <v>0.2</v>
       </c>
       <c r="AC42" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AE42" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF42" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="AF42" s="5" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="43" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="F43" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="G43" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I43" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J43" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="K43" s="23" t="s">
         <v>88</v>
@@ -4182,19 +4655,19 @@
         <v>24</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O43" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="P43" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="P43" s="17" t="s">
+      <c r="Q43" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="Q43" s="17" t="s">
+      <c r="R43" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>292</v>
       </c>
       <c r="W43" s="5" t="s">
         <v>37</v>
@@ -4215,18 +4688,18 @@
         <v>0.2</v>
       </c>
       <c r="AC43" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C44" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="G44" s="23" t="s">
         <v>30</v>
@@ -4235,10 +4708,10 @@
         <v>172</v>
       </c>
       <c r="I44" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="K44" s="23" t="s">
         <v>88</v>
@@ -4247,16 +4720,16 @@
         <v>24</v>
       </c>
       <c r="M44" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="O44" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="O44" s="17" t="s">
+      <c r="P44" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="P44" s="17" t="s">
+      <c r="Q44" s="17" t="s">
         <v>298</v>
-      </c>
-      <c r="Q44" s="17" t="s">
-        <v>299</v>
       </c>
       <c r="W44" s="5" t="s">
         <v>37</v>
@@ -4277,24 +4750,27 @@
         <v>0.2</v>
       </c>
       <c r="AC44" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G45" s="21" t="s">
         <v>300</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>302</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
+      <c r="J45" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="11"/>
@@ -4319,19 +4795,19 @@
     </row>
     <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>307</v>
-      </c>
       <c r="F46" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G46" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>136</v>
@@ -4346,16 +4822,16 @@
         <v>24</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O46" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="P46" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q46" s="17" t="s">
         <v>308</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q46" s="17" t="s">
-        <v>310</v>
       </c>
       <c r="W46" s="5" t="s">
         <v>37</v>
@@ -4381,19 +4857,19 @@
     </row>
     <row r="47" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G47" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>136</v>
@@ -4408,16 +4884,16 @@
         <v>24</v>
       </c>
       <c r="M47" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="O47" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="O47" s="17" t="s">
+      <c r="P47" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q47" s="17" t="s">
         <v>316</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q47" s="17" t="s">
-        <v>318</v>
       </c>
       <c r="W47" s="5" t="s">
         <v>37</v>
@@ -4443,19 +4919,19 @@
     </row>
     <row r="48" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>321</v>
       </c>
       <c r="G48" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>71</v>
@@ -4473,16 +4949,16 @@
         <v>168</v>
       </c>
       <c r="O48" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="P48" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q48" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="P48" s="17" t="s">
+      <c r="S48" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="Q48" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="S48" s="5" t="s">
-        <v>325</v>
       </c>
       <c r="W48" s="5" t="s">
         <v>37</v>
@@ -4501,6 +4977,285 @@
       </c>
       <c r="AB48" s="10">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B49" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="P49" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q49" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="R49" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="W49" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y49" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Z49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA49" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC49" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B50" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="M50" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="R50" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="W50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y50" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Z50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA50" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC50" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B51" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K51" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="M51" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="W51" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X51" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y51" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Z51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA51" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC51" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K52" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="M52" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="W52" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X52" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y52" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Z52" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA52" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC52" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B53" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K53" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="O53" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="P53" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q53" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="S53" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="W53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y53" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="Z53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA53" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC53" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4541,10 +5296,533 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="16.5546875" style="27" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+    </row>
+    <row r="8" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+    </row>
+    <row r="9" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+    </row>
+    <row r="10" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="O10" s="30"/>
+    </row>
+    <row r="11" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="O11" s="30"/>
+    </row>
+    <row r="12" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="O12" s="30"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+    </row>
+    <row r="18" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+    </row>
+    <row r="19" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+    </row>
+    <row r="20" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="J22" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+    </row>
+    <row r="24" spans="2:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="47" t="s">
+        <v>404</v>
+      </c>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B24:O24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4555,13 +5833,13 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -4580,7 +5858,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -4596,15 +5874,15 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" t="s">
         <v>146</v>
@@ -4615,7 +5893,7 @@
         <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -4628,7 +5906,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F9" t="s">
         <v>71</v>
@@ -4636,23 +5914,23 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
@@ -4660,10 +5938,10 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -4671,55 +5949,40 @@
         <v>135</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>334</v>
-      </c>
-      <c r="F15" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>335</v>
-      </c>
-      <c r="F16" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>306</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>172</v>
       </c>
-      <c r="F18" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="F19" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Struggle crit values for Abadon Armor and new modifier
- explicitly set struggle crit values for abadon armor;
- added new modifier CREG (restores DD health when its condition worsenes). It doesn't work as I expected, but it looks ok.
</commit_message>
<xml_diff>
--- a/docs/UD_Modifiers.xlsx
+++ b/docs/UD_Modifiers.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="411">
   <si>
     <t>Name</t>
   </si>
@@ -1512,6 +1512,24 @@
       <t xml:space="preserve"> - Modifiers have presets for the Patcher and can appear on a random device;
 A*_ - Modifiers are used on Abadon armor</t>
     </r>
+  </si>
+  <si>
+    <t>Self Repair</t>
+  </si>
+  <si>
+    <t>Restores the health of the device when its condition has worsened</t>
+  </si>
+  <si>
+    <t>0,100,0,1,,,,1,S,10,25</t>
+  </si>
+  <si>
+    <t>0,100,0,1,,,,1,S,25,75</t>
+  </si>
+  <si>
+    <t>0,100,0,1,,,,1,S,100,100</t>
+  </si>
+  <si>
+    <t>CREG</t>
   </si>
 </sst>
 </file>
@@ -1811,13 +1829,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1835,7 +1850,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1843,6 +1858,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2131,13 +2149,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AF53"/>
+  <dimension ref="B2:AF54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2172,137 +2190,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="37" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="38" t="s">
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="AF2" s="38" t="s">
+      <c r="AF2" s="36" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="43" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="42" t="s">
         <v>340</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="43" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="45" t="s">
+      <c r="N3" s="43"/>
+      <c r="O3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="38" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="S3" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="T3" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="38" t="s">
+      <c r="U3" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="37" t="s">
+      <c r="W3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="46" t="s">
+      <c r="X3" s="43"/>
+      <c r="Y3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="37" t="s">
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37" t="s">
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
     </row>
     <row r="4" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="37"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2318,11 +2336,11 @@
       <c r="Q4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
       <c r="W4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2347,8 +2365,8 @@
       <c r="AD4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -5258,9 +5276,82 @@
         <v>107</v>
       </c>
     </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K54" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="O54" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="P54" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q54" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="W54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y54" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="Z54" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA54" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AC54" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B5:AF48"/>
   <mergeCells count="27">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="K2:AD2"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="AF2:AF4"/>
     <mergeCell ref="AE2:AE4"/>
     <mergeCell ref="D2:F2"/>
@@ -5277,17 +5368,6 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="K2:AD2"/>
-    <mergeCell ref="K3:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5299,7 +5379,7 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5388,7 +5468,9 @@
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+      <c r="M4" s="34" t="s">
+        <v>410</v>
+      </c>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>

</xml_diff>

<commit_message>
Restored missing modifiers in esp
- added new info strings in MCM
</commit_message>
<xml_diff>
--- a/docs/UD_Modifiers.xlsx
+++ b/docs/UD_Modifiers.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="412">
   <si>
     <t>Name</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>Destroy</t>
-  </si>
-  <si>
-    <t>Fragile</t>
   </si>
   <si>
     <t>CLO</t>
@@ -586,12 +583,6 @@
   </si>
   <si>
     <t>BoundWeapon</t>
-  </si>
-  <si>
-    <t>CMB WEAPON</t>
-  </si>
-  <si>
-    <t>WEAPON</t>
   </si>
   <si>
     <t>zad_DeviousGloves</t>
@@ -1530,6 +1521,18 @@
   </si>
   <si>
     <t>CREG</t>
+  </si>
+  <si>
+    <t>Auto destroy</t>
+  </si>
+  <si>
+    <t>WPN</t>
+  </si>
+  <si>
+    <t>CMB WPN</t>
+  </si>
+  <si>
+    <t>ITEM+ ALCO</t>
   </si>
 </sst>
 </file>
@@ -1829,10 +1832,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1850,7 +1856,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1858,9 +1864,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2152,10 +2155,10 @@
   <dimension ref="B2:AF54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="P36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomRight" activeCell="Z55" sqref="Z55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,151 +2179,150 @@
     <col min="15" max="17" width="31" style="17" customWidth="1"/>
     <col min="18" max="18" width="28.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="26.21875" style="5" customWidth="1"/>
+    <col min="20" max="22" width="12.21875" style="5" customWidth="1"/>
     <col min="23" max="24" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.88671875" style="10" customWidth="1"/>
-    <col min="29" max="29" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.33203125" style="5" customWidth="1"/>
+    <col min="29" max="30" width="27.33203125" style="5" customWidth="1"/>
     <col min="31" max="31" width="14.6640625" style="5" customWidth="1"/>
     <col min="32" max="32" width="108.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="43" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="36" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF2" s="36" t="s">
-        <v>95</v>
+      <c r="K2" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF2" s="38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="42" t="s">
-        <v>340</v>
-      </c>
-      <c r="E3" s="43" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" s="43" t="s">
+      <c r="J3" s="37"/>
+      <c r="K3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="44" t="s">
+      <c r="N3" s="37"/>
+      <c r="O3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="36" t="s">
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="36" t="s">
+      <c r="V3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="43" t="s">
+      <c r="W3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="45" t="s">
+      <c r="X3" s="37"/>
+      <c r="Y3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="43" t="s">
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43" t="s">
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
     </row>
     <row r="4" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="43"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="37"/>
       <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2336,11 +2338,11 @@
       <c r="Q4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
       <c r="W4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>16</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="AA4" s="6" t="s">
         <v>16</v>
@@ -2365,8 +2367,8 @@
       <c r="AD4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
     </row>
     <row r="5" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -2465,7 +2467,7 @@
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>54</v>
@@ -2486,7 +2488,7 @@
         <v>23</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>24</v>
@@ -2545,19 +2547,19 @@
         <v>48</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>37</v>
@@ -2604,22 +2606,22 @@
         <v>48</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="W8" s="5" t="s">
         <v>37</v>
@@ -2645,7 +2647,7 @@
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>408</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>55</v>
@@ -2682,36 +2684,36 @@
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>59</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>60</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="Q10" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="Q10" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="W10" s="5" t="s">
         <v>37</v>
@@ -2732,45 +2734,45 @@
         <v>0.2</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="K11" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W11" s="5" t="s">
         <v>37</v>
@@ -2779,7 +2781,7 @@
         <v>37</v>
       </c>
       <c r="Y11" s="8">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>38</v>
@@ -2791,48 +2793,48 @@
         <v>0.2</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="O12" s="17" t="s">
+      <c r="P12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="Q12" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="Q12" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="W12" s="5" t="s">
         <v>37</v>
@@ -2853,18 +2855,18 @@
         <v>0.2</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>30</v>
@@ -2873,25 +2875,25 @@
         <v>46</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="K13" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="W13" s="5" t="s">
         <v>37</v>
@@ -2900,7 +2902,7 @@
         <v>37</v>
       </c>
       <c r="Y13" s="8">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>38</v>
@@ -2912,18 +2914,18 @@
         <v>0.2</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>30</v>
@@ -2932,29 +2934,29 @@
         <v>46</v>
       </c>
       <c r="I14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>73</v>
-      </c>
       <c r="P14" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q14" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Q14" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="W14" s="5" t="s">
         <v>37</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>37</v>
       </c>
       <c r="Y14" s="8">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="Z14" s="5" t="s">
         <v>37</v>
@@ -2974,35 +2976,35 @@
         <v>0.2</v>
       </c>
       <c r="AC14" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="G15" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O15" s="17">
         <v>1</v>
@@ -3032,32 +3034,32 @@
         <v>0.3</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="G16" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>24</v>
@@ -3090,21 +3092,21 @@
         <v>0.2</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="G17" s="23" t="s">
         <v>30</v>
@@ -3113,28 +3115,28 @@
         <v>27</v>
       </c>
       <c r="I17" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="K17" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O17" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="P17" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="P17" s="17" t="s">
+      <c r="Q17" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="Q17" s="17" t="s">
+      <c r="S17" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="W17" s="5" t="s">
         <v>37</v>
@@ -3155,18 +3157,18 @@
         <v>0.2</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>30</v>
@@ -3181,19 +3183,19 @@
         <v>23</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O18" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="P18" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="Q18" s="17" t="s">
         <v>112</v>
-      </c>
-      <c r="Q18" s="17" t="s">
-        <v>113</v>
       </c>
       <c r="W18" s="5" t="s">
         <v>37</v>
@@ -3214,41 +3216,41 @@
         <v>0.2</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="F19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>116</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O19" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="P19" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="P19" s="17" t="s">
+      <c r="Q19" s="17" t="s">
         <v>120</v>
-      </c>
-      <c r="Q19" s="17" t="s">
-        <v>121</v>
       </c>
       <c r="W19" s="5" t="s">
         <v>37</v>
@@ -3269,18 +3271,18 @@
         <v>0.2</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>30</v>
@@ -3289,10 +3291,10 @@
         <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -3318,21 +3320,21 @@
     </row>
     <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="G21" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -3356,48 +3358,48 @@
       <c r="AD21" s="11"/>
       <c r="AE21" s="11"/>
       <c r="AF21" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="K22" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O22" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="P22" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="P22" s="17" t="s">
+      <c r="Q22" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="Q22" s="17" t="s">
-        <v>141</v>
-      </c>
       <c r="S22" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="W22" s="5" t="s">
         <v>37</v>
@@ -3406,7 +3408,7 @@
         <v>37</v>
       </c>
       <c r="Y22" s="8">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="Z22" s="5" t="s">
         <v>38</v>
@@ -3420,46 +3422,46 @@
     </row>
     <row r="23" spans="2:32" ht="72" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="K23" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O23" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="P23" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="P23" s="17" t="s">
+      <c r="Q23" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="S23" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="W23" s="5" t="s">
         <v>37</v>
@@ -3480,18 +3482,18 @@
         <v>0.2</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>30</v>
@@ -3500,28 +3502,28 @@
         <v>46</v>
       </c>
       <c r="I24" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="K24" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="P24" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="P24" s="17" t="s">
+      <c r="Q24" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="Q24" s="17" t="s">
-        <v>158</v>
-      </c>
       <c r="S24" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W24" s="5" t="s">
         <v>37</v>
@@ -3542,51 +3544,51 @@
         <v>0.2</v>
       </c>
       <c r="AC24" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>163</v>
-      </c>
       <c r="K25" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O25" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="P25" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="Q25" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="Q25" s="17" t="s">
+      <c r="S25" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="S25" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="W25" s="5" t="s">
         <v>37</v>
@@ -3609,46 +3611,46 @@
     </row>
     <row r="26" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="K26" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O26" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="P26" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="P26" s="17" t="s">
+      <c r="Q26" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="Q26" s="17" t="s">
-        <v>176</v>
-      </c>
       <c r="S26" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W26" s="5" t="s">
         <v>37</v>
@@ -3671,36 +3673,36 @@
     </row>
     <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="21" t="s">
         <v>179</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>180</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="5" t="s">
-        <v>181</v>
+        <v>410</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="W27" s="5" t="s">
         <v>37</v>
@@ -3721,54 +3723,54 @@
         <v>0.2</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>182</v>
+        <v>409</v>
       </c>
       <c r="AD27" s="5" t="s">
-        <v>182</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N28" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q28" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="O28" s="17" t="s">
+      <c r="S28" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q28" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="S28" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="W28" s="5" t="s">
         <v>37</v>
@@ -3791,46 +3793,46 @@
     </row>
     <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="K29" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N29" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q29" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="O29" s="17" t="s">
+      <c r="S29" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="P29" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q29" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="S29" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="W29" s="5" t="s">
         <v>37</v>
@@ -3853,13 +3855,13 @@
     </row>
     <row r="30" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G30" s="23" t="s">
         <v>30</v>
@@ -3868,31 +3870,31 @@
         <v>46</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>102</v>
+        <v>411</v>
       </c>
       <c r="K30" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="W30" s="5" t="s">
         <v>37</v>
@@ -3913,18 +3915,18 @@
         <v>0.2</v>
       </c>
       <c r="AC30" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>30</v>
@@ -3936,22 +3938,22 @@
         <v>47</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="W31" s="5" t="s">
         <v>37</v>
@@ -3972,21 +3974,21 @@
         <v>0.2</v>
       </c>
       <c r="AC31" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AD31" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>30</v>
@@ -3998,25 +4000,25 @@
         <v>47</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="K32" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>53</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="Q32" s="17" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="W32" s="5" t="s">
         <v>37</v>
@@ -4037,48 +4039,48 @@
         <v>0.2</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AD32" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P33" s="17" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="W33" s="5" t="s">
         <v>37</v>
@@ -4099,51 +4101,51 @@
         <v>0.2</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AD33" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L34" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="P34" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="P34" s="17" t="s">
-        <v>224</v>
-      </c>
       <c r="Q34" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W34" s="5" t="s">
         <v>37</v>
@@ -4164,27 +4166,27 @@
         <v>0.2</v>
       </c>
       <c r="AC34" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AD34" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>47</v>
@@ -4193,19 +4195,19 @@
         <v>48</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P35" s="17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="Q35" s="17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="W35" s="5" t="s">
         <v>37</v>
@@ -4226,24 +4228,24 @@
         <v>0.2</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>47</v>
@@ -4252,22 +4254,22 @@
         <v>48</v>
       </c>
       <c r="K36" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P36" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q36" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="W36" s="5" t="s">
         <v>37</v>
@@ -4288,30 +4290,30 @@
         <v>0.2</v>
       </c>
       <c r="AC36" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G37" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
@@ -4337,13 +4339,13 @@
     </row>
     <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>249</v>
-      </c>
       <c r="F38" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G38" s="23" t="s">
         <v>30</v>
@@ -4352,28 +4354,28 @@
         <v>46</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O38" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="P38" s="17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Q38" s="17" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="W38" s="5" t="s">
         <v>37</v>
@@ -4394,18 +4396,18 @@
         <v>0.2</v>
       </c>
       <c r="AC38" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G39" s="23" t="s">
         <v>30</v>
@@ -4414,28 +4416,28 @@
         <v>46</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="P39" s="17" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Q39" s="17" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="W39" s="5" t="s">
         <v>37</v>
@@ -4456,44 +4458,44 @@
         <v>0.2</v>
       </c>
       <c r="AC39" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="P40" s="17" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="Q40" s="17" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="W40" s="19" t="s">
         <v>38</v>
@@ -4514,18 +4516,18 @@
         <v>0.2</v>
       </c>
       <c r="AF40" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G41" s="23" t="s">
         <v>30</v>
@@ -4534,13 +4536,13 @@
         <v>46</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>24</v>
@@ -4573,21 +4575,21 @@
         <v>0.2</v>
       </c>
       <c r="AC41" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AF41" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G42" s="23" t="s">
         <v>30</v>
@@ -4596,25 +4598,25 @@
         <v>27</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="P42" s="17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="W42" s="5" t="s">
         <v>37</v>
@@ -4635,57 +4637,57 @@
         <v>0.2</v>
       </c>
       <c r="AC42" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AE42" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="AF42" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G43" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="O43" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="P43" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q43" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="R43" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="P43" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q43" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="W43" s="5" t="s">
         <v>37</v>
@@ -4706,48 +4708,48 @@
         <v>0.2</v>
       </c>
       <c r="AC43" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G44" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K44" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M44" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="O44" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="P44" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q44" s="17" t="s">
         <v>295</v>
-      </c>
-      <c r="O44" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q44" s="17" t="s">
-        <v>298</v>
       </c>
       <c r="W44" s="5" t="s">
         <v>37</v>
@@ -4768,26 +4770,26 @@
         <v>0.2</v>
       </c>
       <c r="AC44" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
@@ -4813,43 +4815,43 @@
     </row>
     <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G46" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I46" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J46" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="K46" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="P46" s="17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="Q46" s="17" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="W46" s="5" t="s">
         <v>37</v>
@@ -4870,48 +4872,48 @@
         <v>0.2</v>
       </c>
       <c r="AC46" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>313</v>
-      </c>
       <c r="F47" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G47" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I47" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J47" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J47" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="K47" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M47" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="O47" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="P47" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="O47" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>315</v>
-      </c>
       <c r="Q47" s="17" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="W47" s="5" t="s">
         <v>37</v>
@@ -4932,51 +4934,51 @@
         <v>0.2</v>
       </c>
       <c r="AC47" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G48" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J48" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="K48" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O48" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="P48" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q48" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="S48" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="P48" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q48" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="S48" s="5" t="s">
-        <v>323</v>
       </c>
       <c r="W48" s="5" t="s">
         <v>37</v>
@@ -4999,48 +5001,52 @@
     </row>
     <row r="49" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>354</v>
+        <v>402</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>353</v>
+        <v>403</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
+        <v>407</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="J49" s="5" t="s">
-        <v>355</v>
+        <v>48</v>
       </c>
       <c r="K49" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="N49" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="O49" s="17" t="s">
-        <v>357</v>
+        <v>404</v>
       </c>
       <c r="P49" s="17" t="s">
-        <v>357</v>
+        <v>405</v>
       </c>
       <c r="Q49" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="R49" s="5" t="s">
-        <v>359</v>
+        <v>406</v>
       </c>
       <c r="W49" s="5" t="s">
         <v>37</v>
       </c>
       <c r="X49" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y49" s="8">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="Z49" s="5" t="s">
         <v>38</v>
@@ -5052,47 +5058,53 @@
         <v>0.2</v>
       </c>
       <c r="AC49" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>300</v>
+        <v>115</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="5" t="s">
-        <v>299</v>
+        <v>352</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="M50" s="15" t="s">
-        <v>367</v>
+        <v>24</v>
+      </c>
+      <c r="O50" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="P50" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q50" s="17" t="s">
+        <v>355</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="W50" s="5" t="s">
         <v>37</v>
       </c>
       <c r="X50" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y50" s="8">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Z50" s="5" t="s">
         <v>38</v>
@@ -5104,38 +5116,38 @@
         <v>0.2</v>
       </c>
       <c r="AC50" s="5" t="s">
-        <v>299</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="K51" s="24" t="s">
-        <v>89</v>
+        <v>296</v>
+      </c>
+      <c r="K51" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="R51" s="5" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="W51" s="5" t="s">
         <v>37</v>
@@ -5156,38 +5168,38 @@
         <v>0.2</v>
       </c>
       <c r="AC51" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="K52" s="33" t="s">
-        <v>364</v>
+        <v>296</v>
+      </c>
+      <c r="K52" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="M52" s="15" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="W52" s="5" t="s">
         <v>37</v>
@@ -5208,51 +5220,38 @@
         <v>0.2</v>
       </c>
       <c r="AC52" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="53" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>101</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
       <c r="J53" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K53" s="23" t="s">
-        <v>88</v>
+        <v>296</v>
+      </c>
+      <c r="K53" s="33" t="s">
+        <v>361</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="O53" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="P53" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q53" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="S53" s="5" t="s">
-        <v>352</v>
+        <v>367</v>
+      </c>
+      <c r="M53" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="R53" s="5" t="s">
+        <v>368</v>
       </c>
       <c r="W53" s="5" t="s">
         <v>37</v>
@@ -5261,10 +5260,10 @@
         <v>37</v>
       </c>
       <c r="Y53" s="8">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Z53" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA53" s="9">
         <v>0</v>
@@ -5273,48 +5272,51 @@
         <v>0.2</v>
       </c>
       <c r="AC53" s="5" t="s">
-        <v>107</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
-        <v>405</v>
+        <v>344</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>406</v>
+        <v>345</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>410</v>
+        <v>343</v>
       </c>
       <c r="G54" s="23" t="s">
         <v>30</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>325</v>
+        <v>69</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N54" s="5" t="s">
-        <v>168</v>
+      <c r="M54" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>407</v>
+        <v>347</v>
       </c>
       <c r="P54" s="17" t="s">
-        <v>408</v>
+        <v>347</v>
       </c>
       <c r="Q54" s="17" t="s">
-        <v>409</v>
+        <v>348</v>
+      </c>
+      <c r="S54" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="W54" s="5" t="s">
         <v>37</v>
@@ -5326,7 +5328,7 @@
         <v>0.15</v>
       </c>
       <c r="Z54" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA54" s="9">
         <v>0</v>
@@ -5335,23 +5337,12 @@
         <v>0.2</v>
       </c>
       <c r="AC54" s="5" t="s">
-        <v>215</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B5:AF48"/>
   <mergeCells count="27">
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="K2:AD2"/>
-    <mergeCell ref="K3:K4"/>
     <mergeCell ref="AF2:AF4"/>
     <mergeCell ref="AE2:AE4"/>
     <mergeCell ref="D2:F2"/>
@@ -5368,6 +5359,17 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="K2:AD2"/>
+    <mergeCell ref="K3:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5392,51 +5394,51 @@
   <sheetData>
     <row r="2" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>374</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>335</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>379</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>377</v>
-      </c>
       <c r="N2" s="25" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5446,7 +5448,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
       <c r="J3" s="34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
@@ -5456,7 +5458,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5469,7 +5471,7 @@
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
       <c r="M4" s="34" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
@@ -5483,10 +5485,10 @@
         <v>22</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -5500,7 +5502,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="29" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5518,13 +5520,13 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="34" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
@@ -5538,7 +5540,7 @@
     </row>
     <row r="8" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
@@ -5547,10 +5549,10 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="J8" s="31" t="s">
         <v>395</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>398</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -5560,36 +5562,36 @@
     </row>
     <row r="9" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="34" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="35" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="31" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
     <row r="10" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="29" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -5597,23 +5599,23 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
       <c r="I10" s="31" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="O10" s="30"/>
     </row>
     <row r="11" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="29" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -5621,23 +5623,23 @@
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
       <c r="I11" s="31" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="31" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="O11" s="30"/>
     </row>
     <row r="12" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -5645,20 +5647,20 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="31" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="31" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="O12" s="30"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="29" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -5676,7 +5678,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="29" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
@@ -5694,10 +5696,10 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -5714,7 +5716,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -5723,10 +5725,10 @@
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
@@ -5736,7 +5738,7 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -5754,10 +5756,10 @@
     </row>
     <row r="18" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="29" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
@@ -5766,7 +5768,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
       <c r="J18" s="34" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -5776,19 +5778,19 @@
     </row>
     <row r="19" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="34" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>
       <c r="I19" s="30"/>
       <c r="J19" s="31" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -5802,37 +5804,37 @@
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
       <c r="M20" s="31" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="29" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -5850,21 +5852,21 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
       <c r="G22" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="30" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
@@ -5874,7 +5876,7 @@
     </row>
     <row r="24" spans="2:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="47" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
@@ -5915,13 +5917,13 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -5929,10 +5931,10 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -5940,7 +5942,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -5951,68 +5953,68 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F11" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
@@ -6020,38 +6022,38 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.3">
@@ -6061,12 +6063,12 @@
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>